<commit_message>
GUI to configurate the scanner.
</commit_message>
<xml_diff>
--- a/MemoryMap/Scaner.xlsx
+++ b/MemoryMap/Scaner.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597AF32-36DD-4F85-8D67-5DF7A5711ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scanner" sheetId="4" r:id="rId1"/>
@@ -17,12 +18,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Stantion</t>
   </si>
@@ -295,9 +296,6 @@
   </si>
   <si>
     <t>CS Part no</t>
-  </si>
-  <si>
-    <t>D7100-D7103</t>
   </si>
   <si>
     <t>D7000</t>
@@ -327,8 +325,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,7 +362,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +402,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -502,13 +506,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -555,7 +568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,9 +600,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,6 +652,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -796,14 +845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -815,7 +864,7 @@
     <col min="13" max="13" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +899,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1">
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>3</v>
       </c>
@@ -891,7 +940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="22.5" customHeight="1">
+    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
@@ -914,7 +963,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="22.5" customHeight="1">
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>7</v>
       </c>
@@ -955,7 +1004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="22.5" customHeight="1">
+    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>9</v>
       </c>
@@ -996,7 +1045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="22.5" customHeight="1">
+    <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="8" t="s">
@@ -1019,7 +1068,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" ht="22.5" customHeight="1">
+    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>11</v>
       </c>
@@ -1060,7 +1109,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="22.5" customHeight="1">
+    <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>16</v>
       </c>
@@ -1101,7 +1150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="22.5" customHeight="1">
+    <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>19</v>
       </c>
@@ -1140,7 +1189,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="22.5" customHeight="1">
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>1</v>
       </c>
@@ -1150,33 +1199,31 @@
       <c r="C10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="J10" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1195,36 +1242,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>